<commit_message>
Chamada do dia 27
</commit_message>
<xml_diff>
--- a/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
+++ b/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="124">
   <si>
     <t xml:space="preserve">ALUNOS</t>
   </si>
@@ -803,11 +803,11 @@
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="G3" activeCellId="0" sqref="G3:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -954,8 +954,12 @@
       <c r="F3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="9"/>
@@ -996,8 +1000,12 @@
       <c r="F4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="9"/>
@@ -1038,8 +1046,12 @@
       <c r="F5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="9"/>
@@ -1080,8 +1092,12 @@
       <c r="F6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="G6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="9"/>
@@ -1122,8 +1138,12 @@
       <c r="F7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="9"/>
@@ -1164,8 +1184,12 @@
       <c r="F8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="9"/>
@@ -1206,8 +1230,12 @@
       <c r="F9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="9"/>
@@ -1248,8 +1276,12 @@
       <c r="F10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="9"/>
@@ -1290,8 +1322,12 @@
       <c r="F11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="9"/>
@@ -1332,8 +1368,12 @@
       <c r="F12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="9"/>
@@ -1374,8 +1414,12 @@
       <c r="F13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="G13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="9"/>
@@ -1416,8 +1460,12 @@
       <c r="F14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="9"/>
@@ -1458,8 +1506,12 @@
       <c r="F15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="9"/>
@@ -1500,8 +1552,12 @@
       <c r="F16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="9"/>
@@ -1542,8 +1598,12 @@
       <c r="F17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="9"/>
@@ -1584,8 +1644,12 @@
       <c r="F18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="G18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="9"/>
@@ -1626,8 +1690,12 @@
       <c r="F19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="9"/>
@@ -1668,8 +1736,12 @@
       <c r="F20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="G20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="9"/>
@@ -1710,8 +1782,12 @@
       <c r="F21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="G21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="9"/>
@@ -1752,8 +1828,12 @@
       <c r="F22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="G22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="9"/>
@@ -1794,8 +1874,12 @@
       <c r="F23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="G23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="9"/>
@@ -1836,8 +1920,12 @@
       <c r="F24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="G24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="9"/>
@@ -1878,8 +1966,12 @@
       <c r="F25" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="G25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="9"/>
@@ -1920,8 +2012,12 @@
       <c r="F26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="G26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="9"/>
@@ -1962,8 +2058,12 @@
       <c r="F27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="G27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="9"/>
@@ -2004,8 +2104,12 @@
       <c r="F28" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="9"/>
@@ -2046,8 +2150,12 @@
       <c r="F29" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="G29" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="9"/>
@@ -2084,8 +2192,12 @@
       <c r="F30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="G30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="9"/>
@@ -2126,8 +2238,12 @@
       <c r="F31" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
       <c r="K31" s="9"/>
@@ -2168,8 +2284,12 @@
       <c r="F32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+      <c r="G32" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
       <c r="K32" s="9"/>
@@ -2210,8 +2330,12 @@
       <c r="F33" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
+      <c r="G33" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
       <c r="K33" s="9"/>
@@ -2252,8 +2376,12 @@
       <c r="F34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
+      <c r="G34" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
       <c r="K34" s="9"/>
@@ -2294,8 +2422,12 @@
       <c r="F35" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="G35" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="9"/>
@@ -2336,8 +2468,12 @@
       <c r="F36" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+      <c r="G36" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="K36" s="9"/>
@@ -2374,8 +2510,12 @@
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="G37" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
       <c r="K37" s="9"/>
@@ -2416,8 +2556,12 @@
       <c r="F38" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="G38" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
       <c r="K38" s="9"/>
@@ -2458,8 +2602,12 @@
       <c r="F39" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="G39" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="9"/>
@@ -2500,8 +2648,12 @@
       <c r="F40" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="G40" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
       <c r="K40" s="9"/>
@@ -2542,8 +2694,12 @@
       <c r="F41" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="G41" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="9"/>
@@ -2580,8 +2736,12 @@
       <c r="F42" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="G42" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
       <c r="K42" s="9"/>
@@ -2622,8 +2782,12 @@
       <c r="F43" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="G43" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
       <c r="K43" s="9"/>
@@ -2664,8 +2828,12 @@
       <c r="F44" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="G44" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
       <c r="K44" s="9"/>
@@ -2706,8 +2874,12 @@
       <c r="F45" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+      <c r="G45" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="K45" s="9"/>
@@ -2748,8 +2920,12 @@
       <c r="F46" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
+      <c r="G46" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
       <c r="K46" s="9"/>
@@ -2790,8 +2966,12 @@
       <c r="F47" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
+      <c r="G47" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
       <c r="K47" s="9"/>
@@ -2832,8 +3012,12 @@
       <c r="F48" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
+      <c r="G48" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
       <c r="K48" s="9"/>
@@ -2874,8 +3058,12 @@
       <c r="F49" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
+      <c r="G49" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="14"/>

</xml_diff>

<commit_message>
Iniciando a construção do nosso arquivo index.js
</commit_message>
<xml_diff>
--- a/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
+++ b/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="124">
   <si>
     <t xml:space="preserve">ALUNOS</t>
   </si>
@@ -803,11 +803,11 @@
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="G3" activeCellId="0" sqref="G3:H49"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -960,8 +960,12 @@
       <c r="H3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="10"/>
@@ -1006,8 +1010,12 @@
       <c r="H4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="10"/>
@@ -1052,8 +1060,12 @@
       <c r="H5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="10"/>
@@ -1098,8 +1110,12 @@
       <c r="H6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="10"/>
@@ -1144,8 +1160,12 @@
       <c r="H7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="10"/>
@@ -1190,8 +1210,12 @@
       <c r="H8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="10"/>
@@ -1236,8 +1260,12 @@
       <c r="H9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="10"/>
@@ -1282,8 +1310,12 @@
       <c r="H10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="10"/>
@@ -1328,8 +1360,12 @@
       <c r="H11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="10"/>
@@ -1374,8 +1410,12 @@
       <c r="H12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="10"/>
@@ -1420,8 +1460,12 @@
       <c r="H13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="I13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="10"/>
@@ -1466,8 +1510,12 @@
       <c r="H14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="10"/>
@@ -1512,8 +1560,12 @@
       <c r="H15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="10"/>
@@ -1558,8 +1610,12 @@
       <c r="H16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="10"/>
@@ -1604,8 +1660,12 @@
       <c r="H17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="I17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="10"/>
@@ -1650,8 +1710,12 @@
       <c r="H18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="I18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="10"/>
@@ -1696,8 +1760,12 @@
       <c r="H19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="I19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="10"/>
@@ -1742,8 +1810,12 @@
       <c r="H20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="I20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="10"/>
@@ -1788,8 +1860,12 @@
       <c r="H21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="I21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="10"/>
@@ -1834,8 +1910,12 @@
       <c r="H22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="I22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="10"/>
@@ -1880,8 +1960,12 @@
       <c r="H23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="I23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="10"/>
@@ -1926,8 +2010,12 @@
       <c r="H24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="I24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="10"/>
@@ -2018,8 +2106,12 @@
       <c r="H26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="I26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="10"/>
@@ -2064,8 +2156,12 @@
       <c r="H27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
+      <c r="I27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="10"/>
@@ -2110,8 +2206,12 @@
       <c r="H28" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="I28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>
@@ -2156,8 +2256,12 @@
       <c r="H29" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="I29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="10"/>
@@ -2198,8 +2302,12 @@
       <c r="H30" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="I30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="10"/>
@@ -2244,8 +2352,12 @@
       <c r="H31" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="I31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="10"/>
@@ -2290,8 +2402,12 @@
       <c r="H32" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
+      <c r="I32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="10"/>
@@ -2336,8 +2452,12 @@
       <c r="H33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
+      <c r="I33" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="10"/>
@@ -2382,8 +2502,12 @@
       <c r="H34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
+      <c r="I34" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
       <c r="M34" s="10"/>
@@ -2428,8 +2552,12 @@
       <c r="H35" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
+      <c r="I35" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
       <c r="M35" s="10"/>
@@ -2474,8 +2602,12 @@
       <c r="H36" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
+      <c r="I36" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="10"/>
@@ -2516,8 +2648,12 @@
       <c r="H37" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="I37" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="10"/>
@@ -2562,8 +2698,12 @@
       <c r="H38" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
+      <c r="I38" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="10"/>
@@ -2608,8 +2748,12 @@
       <c r="H39" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
+      <c r="I39" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="10"/>
@@ -2654,8 +2798,12 @@
       <c r="H40" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
+      <c r="I40" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="10"/>
@@ -2700,8 +2848,12 @@
       <c r="H41" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
+      <c r="I41" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="10"/>
@@ -2742,8 +2894,12 @@
       <c r="H42" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
+      <c r="I42" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
       <c r="M42" s="10"/>
@@ -2788,8 +2944,12 @@
       <c r="H43" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
+      <c r="I43" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="10"/>
@@ -2834,8 +2994,12 @@
       <c r="H44" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
+      <c r="I44" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="10"/>
@@ -2880,8 +3044,12 @@
       <c r="H45" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
+      <c r="I45" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="10"/>
@@ -2926,8 +3094,12 @@
       <c r="H46" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
+      <c r="I46" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="10"/>
@@ -2972,8 +3144,12 @@
       <c r="H47" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
+      <c r="I47" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="10"/>
@@ -3018,8 +3194,12 @@
       <c r="H48" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
+      <c r="I48" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="10"/>
@@ -3064,8 +3244,12 @@
       <c r="H49" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
+      <c r="I49" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="K49" s="14"/>
       <c r="L49" s="14"/>
       <c r="M49" s="15"/>

</xml_diff>

<commit_message>
Fim da primeira semana
</commit_message>
<xml_diff>
--- a/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
+++ b/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="124">
   <si>
     <t xml:space="preserve">ALUNOS</t>
   </si>
@@ -807,7 +807,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3:J49"/>
+      <selection pane="bottomRight" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -966,8 +966,12 @@
       <c r="J3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="K3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="9"/>
@@ -1016,8 +1020,12 @@
       <c r="J4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
+      <c r="K4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="9"/>
@@ -1066,8 +1074,12 @@
       <c r="J5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="K5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="9"/>
@@ -1116,8 +1128,12 @@
       <c r="J6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="K6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="9"/>
@@ -1166,8 +1182,12 @@
       <c r="J7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="K7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="9"/>
@@ -1216,8 +1236,12 @@
       <c r="J8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="K8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="9"/>
@@ -1266,8 +1290,12 @@
       <c r="J9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="K9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="9"/>
@@ -1316,8 +1344,12 @@
       <c r="J10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="K10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="9"/>
@@ -1366,8 +1398,12 @@
       <c r="J11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="9"/>
@@ -1416,8 +1452,12 @@
       <c r="J12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="K12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="9"/>
@@ -1466,8 +1506,12 @@
       <c r="J13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="K13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="9"/>
@@ -1516,8 +1560,12 @@
       <c r="J14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="K14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="9"/>
@@ -1566,8 +1614,12 @@
       <c r="J15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="K15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="9"/>
@@ -1616,8 +1668,12 @@
       <c r="J16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+      <c r="K16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="9"/>
@@ -1666,8 +1722,12 @@
       <c r="J17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+      <c r="K17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="9"/>
@@ -1716,8 +1776,12 @@
       <c r="J18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="K18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="9"/>
@@ -1766,8 +1830,12 @@
       <c r="J19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
+      <c r="K19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="9"/>
@@ -1816,8 +1884,12 @@
       <c r="J20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="K20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="9"/>
@@ -1866,8 +1938,12 @@
       <c r="J21" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
+      <c r="K21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="9"/>
@@ -1916,8 +1992,12 @@
       <c r="J22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
+      <c r="K22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="9"/>
@@ -1966,8 +2046,12 @@
       <c r="J23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
+      <c r="K23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="9"/>
@@ -2016,8 +2100,12 @@
       <c r="J24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="K24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="9"/>
@@ -2112,8 +2200,12 @@
       <c r="J26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
+      <c r="K26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="9"/>
@@ -2162,8 +2254,12 @@
       <c r="J27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
+      <c r="K27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="9"/>
@@ -2212,8 +2308,12 @@
       <c r="J28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
+      <c r="K28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="9"/>
@@ -2262,8 +2362,12 @@
       <c r="J29" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
+      <c r="K29" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="9"/>
@@ -2308,8 +2412,12 @@
       <c r="J30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
+      <c r="K30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
       <c r="O30" s="9"/>
@@ -2358,8 +2466,12 @@
       <c r="J31" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
+      <c r="K31" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
       <c r="O31" s="9"/>
@@ -2408,8 +2520,12 @@
       <c r="J32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
+      <c r="K32" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="9"/>
@@ -2458,8 +2574,12 @@
       <c r="J33" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
+      <c r="K33" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
       <c r="O33" s="9"/>
@@ -2508,8 +2628,12 @@
       <c r="J34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
+      <c r="K34" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="O34" s="9"/>
@@ -2558,8 +2682,12 @@
       <c r="J35" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
+      <c r="K35" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
       <c r="O35" s="9"/>
@@ -2608,8 +2736,12 @@
       <c r="J36" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
+      <c r="K36" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
       <c r="O36" s="9"/>
@@ -2654,8 +2786,12 @@
       <c r="J37" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
+      <c r="K37" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="9"/>
@@ -2704,8 +2840,12 @@
       <c r="J38" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
+      <c r="K38" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
       <c r="O38" s="9"/>
@@ -2754,8 +2894,12 @@
       <c r="J39" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
+      <c r="K39" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
       <c r="O39" s="9"/>
@@ -2804,8 +2948,12 @@
       <c r="J40" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
+      <c r="K40" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="9"/>
@@ -2854,8 +3002,12 @@
       <c r="J41" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
+      <c r="K41" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="9"/>
@@ -2900,8 +3052,12 @@
       <c r="J42" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
+      <c r="K42" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L42" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="9"/>
@@ -2950,8 +3106,12 @@
       <c r="J43" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
+      <c r="K43" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L43" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="9"/>
@@ -3000,8 +3160,12 @@
       <c r="J44" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
+      <c r="K44" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="9"/>
@@ -3050,8 +3214,12 @@
       <c r="J45" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
+      <c r="K45" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
       <c r="O45" s="9"/>
@@ -3100,8 +3268,12 @@
       <c r="J46" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
+      <c r="K46" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
       <c r="O46" s="9"/>
@@ -3150,8 +3322,12 @@
       <c r="J47" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
+      <c r="K47" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="9"/>
@@ -3200,8 +3376,12 @@
       <c r="J48" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
+      <c r="K48" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L48" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="9"/>
@@ -3250,8 +3430,12 @@
       <c r="J49" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
+      <c r="K49" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L49" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
       <c r="O49" s="14"/>

</xml_diff>

<commit_message>
Iniciando o estudo de bootstrap
</commit_message>
<xml_diff>
--- a/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
+++ b/Lista de Presença - AVANADE SE Ciclo I - Erik Johaness.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="124">
   <si>
     <t xml:space="preserve">ALUNOS</t>
   </si>
@@ -712,22 +712,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED135A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -807,7 +791,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L3" activeCellId="0" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="N51" activeCellId="0" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -972,8 +956,12 @@
       <c r="L3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="M3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="10"/>
@@ -1026,8 +1014,12 @@
       <c r="L4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="M4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="10"/>
@@ -1080,8 +1072,12 @@
       <c r="L5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="10"/>
@@ -1134,8 +1130,12 @@
       <c r="L6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="M6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="10"/>
@@ -1188,8 +1188,12 @@
       <c r="L7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
+      <c r="M7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="10"/>
@@ -1242,8 +1246,12 @@
       <c r="L8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
+      <c r="M8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="10"/>
@@ -1296,8 +1304,12 @@
       <c r="L9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="M9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="10"/>
@@ -1350,8 +1362,12 @@
       <c r="L10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
+      <c r="M10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="10"/>
@@ -1404,8 +1420,12 @@
       <c r="L11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
+      <c r="M11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="10"/>
@@ -1458,8 +1478,12 @@
       <c r="L12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
+      <c r="M12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="10"/>
@@ -1512,8 +1536,12 @@
       <c r="L13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+      <c r="M13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="10"/>
@@ -1566,8 +1594,12 @@
       <c r="L14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
+      <c r="M14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
       <c r="Q14" s="10"/>
@@ -1620,8 +1652,12 @@
       <c r="L15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+      <c r="M15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="10"/>
@@ -1674,8 +1710,12 @@
       <c r="L16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+      <c r="M16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="10"/>
@@ -1728,8 +1768,12 @@
       <c r="L17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
+      <c r="M17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="10"/>
@@ -1782,8 +1826,12 @@
       <c r="L18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
+      <c r="M18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="10"/>
@@ -1836,8 +1884,12 @@
       <c r="L19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
+      <c r="M19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="10"/>
@@ -1890,8 +1942,12 @@
       <c r="L20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="M20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="10"/>
@@ -1944,8 +2000,12 @@
       <c r="L21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
+      <c r="M21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="10"/>
@@ -1998,8 +2058,12 @@
       <c r="L22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
+      <c r="M22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="10"/>
@@ -2052,8 +2116,12 @@
       <c r="L23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
+      <c r="M23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="10"/>
@@ -2106,8 +2174,12 @@
       <c r="L24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
+      <c r="M24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="10"/>
@@ -2206,8 +2278,12 @@
       <c r="L26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
+      <c r="M26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
       <c r="Q26" s="10"/>
@@ -2260,8 +2336,12 @@
       <c r="L27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
+      <c r="M27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="10"/>
@@ -2314,8 +2394,12 @@
       <c r="L28" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
+      <c r="M28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="10"/>
@@ -2368,8 +2452,12 @@
       <c r="L29" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
+      <c r="M29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="10"/>
@@ -2418,8 +2506,12 @@
       <c r="L30" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
+      <c r="M30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="10"/>
@@ -2472,8 +2564,12 @@
       <c r="L31" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
+      <c r="M31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="10"/>
@@ -2526,8 +2622,12 @@
       <c r="L32" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
+      <c r="M32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="10"/>
@@ -2580,8 +2680,12 @@
       <c r="L33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
+      <c r="M33" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N33" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="10"/>
@@ -2634,8 +2738,12 @@
       <c r="L34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
+      <c r="M34" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N34" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
       <c r="Q34" s="10"/>
@@ -2688,8 +2796,12 @@
       <c r="L35" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
+      <c r="M35" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="10"/>
@@ -2742,8 +2854,12 @@
       <c r="L36" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
+      <c r="M36" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N36" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="10"/>
@@ -2792,8 +2908,12 @@
       <c r="L37" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
+      <c r="M37" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N37" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="10"/>
@@ -2846,8 +2966,12 @@
       <c r="L38" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
+      <c r="M38" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N38" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="10"/>
@@ -2900,8 +3024,12 @@
       <c r="L39" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
+      <c r="M39" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N39" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
       <c r="Q39" s="10"/>
@@ -2954,8 +3082,12 @@
       <c r="L40" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
+      <c r="M40" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O40" s="9"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="10"/>
@@ -3008,8 +3140,12 @@
       <c r="L41" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
+      <c r="M41" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N41" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="10"/>
@@ -3058,8 +3194,12 @@
       <c r="L42" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
+      <c r="M42" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N42" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="10"/>
@@ -3112,8 +3252,12 @@
       <c r="L43" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
+      <c r="M43" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N43" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="10"/>
@@ -3166,8 +3310,12 @@
       <c r="L44" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
+      <c r="M44" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N44" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="10"/>
@@ -3220,8 +3368,12 @@
       <c r="L45" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
+      <c r="M45" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N45" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="10"/>
@@ -3274,8 +3426,12 @@
       <c r="L46" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
+      <c r="M46" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N46" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O46" s="9"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="10"/>
@@ -3328,8 +3484,12 @@
       <c r="L47" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
+      <c r="M47" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N47" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O47" s="9"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="10"/>
@@ -3382,8 +3542,12 @@
       <c r="L48" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
+      <c r="M48" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N48" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="O48" s="9"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="10"/>
@@ -3436,8 +3600,12 @@
       <c r="L49" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
+      <c r="M49" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N49" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="O49" s="14"/>
       <c r="P49" s="14"/>
       <c r="Q49" s="15"/>
@@ -3464,8 +3632,8 @@
     <hyperlink ref="B22" r:id="rId1" display="j.delmondes.cais@avanade.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>